<commit_message>
fix db and add item moudle
</commit_message>
<xml_diff>
--- a/tools/excel/excel/Global.xlsx
+++ b/tools/excel/excel/Global.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -41,13 +41,22 @@
     <t>int</t>
   </si>
   <si>
+    <t>table</t>
+  </si>
+  <si>
     <t>Id</t>
   </si>
   <si>
     <t>value1</t>
   </si>
   <si>
+    <t>value2</t>
+  </si>
+  <si>
     <t>c/s</t>
+  </si>
+  <si>
+    <t>{{reward_type = 3,item_type = 2,item_count = 1},{reward_type = 4,item_type = 1,item_count = 1000}}</t>
   </si>
 </sst>
 </file>
@@ -60,7 +69,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,22 +85,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -549,19 +545,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -570,131 +575,122 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -702,11 +698,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,56 +1020,71 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.1" customHeight="1" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.1" customHeight="1" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="6.25" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="2" max="3" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:2">
+    <row r="1" ht="16.5" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" ht="16.5" spans="1:2">
+    <row r="2" ht="16.5" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" ht="16.5" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
+    <row r="3" ht="16.5" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:2">
-      <c r="A5" s="5">
+    <row r="5" customHeight="1" spans="1:3">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>